<commit_message>
updating a warning message and MT4511 prereqs
</commit_message>
<xml_diff>
--- a/src/advising/Module_catalogue.xlsx
+++ b/src/advising/Module_catalogue.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/module_catalogue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/src/advising/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A72EBC3-3DBF-D548-9FC8-658C17C7614D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53475DC5-C5B1-C249-9520-84E3398F325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="293">
   <si>
     <t>Module code</t>
   </si>
@@ -912,6 +912,9 @@
   </si>
   <si>
     <t>MT1007 or MT2508 or EC2203 or PH3012 and (co-requisite MT3501 or co-requisite MT3502 or co-requisite MT3503 or co-requisite MT3504 or co-requisite MT3505 or co-requisite MT3506 or co-requisite MT3507 or co-requisite MT3508)</t>
+  </si>
+  <si>
+    <t>co-requisite MT3504</t>
   </si>
 </sst>
 </file>
@@ -1297,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2084,7 @@
         <v>80</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>47</v>
+        <v>292</v>
       </c>
       <c r="H32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added intended pre-requisites for MT45AB and MT45ML, the planned modules to be introduced in 2025-26
</commit_message>
<xml_diff>
--- a/src/advising/Module_catalogue.xlsx
+++ b/src/advising/Module_catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/src/advising/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/dwrj1_st-andrews_ac_uk/Documents/DoT/Advising/Advising-tool/StA_Advising/src/advising/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53475DC5-C5B1-C249-9520-84E3398F325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{53475DC5-C5B1-C249-9520-84E3398F325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B31E7470-6FE8-5443-8083-B7462A25C98E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="50240" windowHeight="19820" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -884,9 +884,6 @@
     <t>Applied Bayesian Methods</t>
   </si>
   <si>
-    <t>TBC</t>
-  </si>
-  <si>
     <t>MT45ML</t>
   </si>
   <si>
@@ -915,6 +912,9 @@
   </si>
   <si>
     <t>co-requisite MT3504</t>
+  </si>
+  <si>
+    <t>MT2501 and MT2503 and MT2508</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1887,7 +1887,7 @@
         <v>80</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -1960,7 +1960,7 @@
         <v>80</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>81</v>
@@ -2084,7 +2084,7 @@
         <v>80</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2423,7 +2423,7 @@
         <v>80</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3028,7 +3028,7 @@
         <v>80</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H72" s="1"/>
     </row>
@@ -3671,16 +3671,16 @@
       <c r="F98" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G98" s="2" t="s">
-        <v>282</v>
+      <c r="G98" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>122</v>
@@ -3694,16 +3694,16 @@
       <c r="F99" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G99" s="2" t="s">
-        <v>282</v>
+      <c r="G99" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>129</v>
@@ -3718,7 +3718,7 @@
         <v>80</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MT4539, MT4537, and MT4530 are temporarily withdrawn
</commit_message>
<xml_diff>
--- a/src/advising/Module_catalogue.xlsx
+++ b/src/advising/Module_catalogue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/dwrj1_st-andrews_ac_uk/Documents/DoT/Advising/Advising-tool/StA_Advising/src/advising/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk263/Projects/StA_Advising/src/advising/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{53475DC5-C5B1-C249-9520-84E3398F325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B31E7470-6FE8-5443-8083-B7462A25C98E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84145898-1FC4-A746-8358-CC0400B61A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="50240" windowHeight="19820" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="294">
   <si>
     <t>Module code</t>
   </si>
@@ -915,6 +915,9 @@
   </si>
   <si>
     <t>MT2501 and MT2503 and MT2508</t>
+  </si>
+  <si>
+    <t>2030/2031</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2317,7 @@
         <v>121</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>122</v>
+        <v>293</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -2364,7 +2367,7 @@
         <v>128</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>129</v>
+        <v>293</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>15</v>
@@ -2387,7 +2390,7 @@
         <v>131</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>129</v>
+        <v>293</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Corrected alternating pattern of MT5864
</commit_message>
<xml_diff>
--- a/src/advising/Module_catalogue.xlsx
+++ b/src/advising/Module_catalogue.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/dwrj1_st-andrews_ac_uk/Documents/DoT/Advising/Advising-tool/StA_Advising/src/advising/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{84145898-1FC4-A746-8358-CC0400B61A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44835840-3BC8-9E44-B22F-F9D6E9AD3CF8}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{84145898-1FC4-A746-8358-CC0400B61A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABD784D5-B4AC-7642-BF28-8CDF43B432A5}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{4F9A127D-94E5-E147-ADFA-9B9D4F5F7BAB}"/>
   </bookViews>
@@ -1309,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692125B0-B9FD-1C45-BA4C-1792B9B50D49}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3502,7 +3502,7 @@
         <v>239</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>11</v>

</xml_diff>